<commit_message>
Se actualiza documento de indicadores kpi
</commit_message>
<xml_diff>
--- a/Diapositivas/Sem-7/IndicadoresSM.xlsx
+++ b/Diapositivas/Sem-7/IndicadoresSM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlberto\Documents\Doctorado\Posdoctorado\ITQ\2024-2\SistemasDeManufactura\Sem-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlberto\Desktop\ITQ\SistemasDeManufactura-2024\Diapositivas\Sem-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81275C-5745-4019-88FE-5D57C7C2308D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEE8AD0-327C-43D6-8406-FB3D125415F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,10 +172,10 @@
     <t>De cumplimiento</t>
   </si>
   <si>
-    <t>Instrucciones: Llena la tabla de KPI's que esta en la Hoja de Excel con nombre KPI, te guiaras con esta hoja y las tablas. Una vez que la termines sube la table completada a tu branch en la carpeta img y da push, recuerda que es parte de la calificación de la segunda unidad.</t>
-  </si>
-  <si>
     <t>OGSM</t>
+  </si>
+  <si>
+    <t>Instrucciones: Llena la tabla OGSM y la de KPI's que está en la Hoja de Excel con nombre KPI, te guiaras con esta hoja y las tablas. Una vez que la termines sube las tablas completadas a tu branch en la carpeta img y da push, recuerda que es parte de la calificación de la segunda unidad.</t>
   </si>
 </sst>
 </file>
@@ -361,6 +361,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,9 +372,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,21 +936,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -1351,43 +1351,43 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
       <c r="L3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="9" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Agrego Avance de mi Proyecto Integrador Excel y Power Point
</commit_message>
<xml_diff>
--- a/Diapositivas/Sem-7/IndicadoresSM.xlsx
+++ b/Diapositivas/Sem-7/IndicadoresSM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlberto\Desktop\ITQ\SistemasDeManufactura-2024\Diapositivas\Sem-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Desktop\ITQ\SistemasDeManufactura-2024\Diapositivas\Sem-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEE8AD0-327C-43D6-8406-FB3D125415F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OGSM" sheetId="1" r:id="rId1"/>
-    <sheet name="KPI" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="KPI" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>Objetivo</t>
   </si>
@@ -176,12 +176,51 @@
   </si>
   <si>
     <t>Instrucciones: Llena la tabla OGSM y la de KPI's que está en la Hoja de Excel con nombre KPI, te guiaras con esta hoja y las tablas. Una vez que la termines sube las tablas completadas a tu branch en la carpeta img y da push, recuerda que es parte de la calificación de la segunda unidad.</t>
+  </si>
+  <si>
+    <t>Que los alumnos del Instituto Tegnologico De Queretaro puedan solucionar problemas con ayuda de de la plataforma de GitHub.</t>
+  </si>
+  <si>
+    <t>100 % del cumplimiento al programa de capacitacion de los alumnos del Instituto Tecnologico De Queretaro.</t>
+  </si>
+  <si>
+    <t>Que los alumnos del ITQ cumplan con el 100% de todas las practicas realizadas en el semestre.</t>
+  </si>
+  <si>
+    <t>Diseñar e implementar un programa de capacitacion para que los alumnos puedan manejar y controlar plataformas como GitHub.</t>
+  </si>
+  <si>
+    <t>PROFESOR.</t>
+  </si>
+  <si>
+    <t>ALUMNO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumplir con todas las aesorias para poder mejorar el manejo de la plataforma Git Hub. </t>
+  </si>
+  <si>
+    <t>Cumplir con la rubrica establecida por el profesor como lo son 20% Asistencia,70%, evaluacion/unidad.</t>
+  </si>
+  <si>
+    <t>calidad</t>
+  </si>
+  <si>
+    <t>costo</t>
+  </si>
+  <si>
+    <t>entrega</t>
+  </si>
+  <si>
+    <t>medio ambiente</t>
+  </si>
+  <si>
+    <t>seguridad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,14 +394,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,7 +416,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -458,7 +581,7 @@
         <xdr:cNvPr id="3" name="Conector recto de flecha 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -511,7 +634,7 @@
         <xdr:cNvPr id="4" name="Conector recto de flecha 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -564,7 +687,7 @@
         <xdr:cNvPr id="7" name="Conector recto de flecha 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -617,7 +740,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -627,6 +750,223 @@
         <a:xfrm flipH="1">
           <a:off x="3143250" y="4143375"/>
           <a:ext cx="2324100" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto de flecha 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1889760" y="1979295"/>
+          <a:ext cx="2526031" cy="1312545"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1072515</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>280035</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>815340</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3480435" y="2192655"/>
+          <a:ext cx="2844165" cy="1042035"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto de flecha 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1022985" y="4303395"/>
+          <a:ext cx="2390775" cy="912495"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto de flecha 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2432685" y="4417695"/>
+          <a:ext cx="2402205" cy="912495"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -917,50 +1257,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="19.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -974,45 +1314,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1026,25 +1366,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="E12" s="17"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
@@ -1058,45 +1398,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1110,25 +1450,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="E22" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>0</v>
       </c>
@@ -1142,45 +1482,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-    </row>
-    <row r="30" spans="2:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="2:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
@@ -1194,25 +1534,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16" t="s">
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="16"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="s">
+      <c r="E32" s="17"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>0</v>
       </c>
@@ -1226,48 +1566,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
@@ -1281,18 +1621,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16" t="s">
+      <c r="C43" s="17"/>
+      <c r="D43" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="16"/>
+      <c r="E43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
@@ -1309,19 +1662,6 @@
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1329,28 +1669,680 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA693FF7-F93C-4941-B739-5CD11833879A}">
-  <dimension ref="B3:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="1">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="17"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +2373,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
       <c r="C4" s="21"/>
       <c r="D4" s="20"/>
@@ -1404,7 +2396,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
@@ -1442,7 +2434,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>38</v>
       </c>
@@ -1478,6 +2470,107 @@
       </c>
       <c r="L6" s="13" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="13">
+        <v>10</v>
+      </c>
+      <c r="I7" s="15">
+        <f>H7</f>
+        <v>10</v>
+      </c>
+      <c r="J7" s="15">
+        <f>H7</f>
+        <v>10</v>
+      </c>
+      <c r="K7" s="15">
+        <f>H7</f>
+        <v>10</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="13">
+        <v>100</v>
+      </c>
+      <c r="I8" s="15">
+        <f>H8</f>
+        <v>100</v>
+      </c>
+      <c r="J8" s="15">
+        <f>H8</f>
+        <v>100</v>
+      </c>
+      <c r="K8" s="15">
+        <f>H8</f>
+        <v>100</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E11" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1491,33 +2584,64 @@
     <mergeCell ref="G3:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="between">
       <formula>99</formula>
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:K6">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
+      <formula>99</formula>
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:K8">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>